<commit_message>
Site updated: 2019-10-17 17:30:30
</commit_message>
<xml_diff>
--- a/2019/09/23/OpenSOC原型图/落地详情.xlsx
+++ b/2019/09/23/OpenSOC原型图/落地详情.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28060" windowHeight="11920" activeTab="5"/>
+    <workbookView windowWidth="28060" windowHeight="11920" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="首页" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,16 @@
     <sheet name="攻击链路分析页" sheetId="4" r:id="rId4"/>
     <sheet name="关联分析页" sheetId="5" r:id="rId5"/>
     <sheet name="用户中心页" sheetId="6" r:id="rId6"/>
+    <sheet name="数据存储" sheetId="7" r:id="rId7"/>
+    <sheet name="大数据平台" sheetId="8" r:id="rId8"/>
+    <sheet name="机器学习平台" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327">
   <si>
     <t>首页（所有告警按钮一律红色小铃铛）</t>
   </si>
@@ -741,7 +744,7 @@
     <t>鼠标悬停群集节点</t>
   </si>
   <si>
-    <t>显示正在遭受攻击的端点IP，按顺序排列，且同时按照IP进行关联到各个其它群集；确认攻击事件红色连接（线的粗细按照登记严重度），疑似事件黄色连接</t>
+    <t>显示正在遭受攻击的端点IP，按顺序排列，且同时按照IP进行关联到各个其它群集；确认攻击事件红色连接（线的粗细按照等级严重度），疑似事件黄色连接</t>
   </si>
   <si>
     <t>后台显示确认攻击事件，和疑似攻击事件</t>
@@ -947,16 +950,70 @@
   <si>
     <t>领导点击审核页面地址，需先登录，再跳转到审核页面，进行审核，点击同意，或拒绝，都会发送邮件给设置维护申请人</t>
   </si>
+  <si>
+    <t>运维指标的数据处理方案：</t>
+  </si>
+  <si>
+    <t>以JSON格式存储一份最初原始各指标内容，以后每次更改指标，只以JSON格式记录更新的指标，前端显示最新更新后的数据</t>
+  </si>
+  <si>
+    <t>考虑使用mongodb存储键值数据</t>
+  </si>
+  <si>
+    <t>对于实时日志数据处理方案：</t>
+  </si>
+  <si>
+    <t>日志处理成JSON格式，存储到Hadoop中，再从Hadoop中抽取JSON数据，进行分析处理，如异常检测，攻击类型检测与确认</t>
+  </si>
+  <si>
+    <t>机器学习部分数据处理，可以考虑使用flink sql，和spark sql</t>
+  </si>
+  <si>
+    <t>对于攻击链路数据处理方案：</t>
+  </si>
+  <si>
+    <t>可以用mongodb，和flink sql等</t>
+  </si>
+  <si>
+    <t>对于关联分析部分的数据处理方案：</t>
+  </si>
+  <si>
+    <t>涉及图存储，考虑使用neo4j来存储关联关系</t>
+  </si>
+  <si>
+    <t>spark</t>
+  </si>
+  <si>
+    <t>flink</t>
+  </si>
+  <si>
+    <t>hadoop</t>
+  </si>
+  <si>
+    <t>spark ml</t>
+  </si>
+  <si>
+    <t>flink ml</t>
+  </si>
+  <si>
+    <t>deeplearning4j</t>
+  </si>
+  <si>
+    <t>angel</t>
+  </si>
+  <si>
+    <t>spark graph</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -974,23 +1031,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1005,14 +1047,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1025,11 +1076,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1038,6 +1089,14 @@
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1051,7 +1110,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1059,7 +1133,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1073,39 +1154,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1120,13 +1177,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,25 +1255,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,115 +1285,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1294,13 +1309,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,17 +1389,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1362,36 +1413,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1411,157 +1438,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1570,9 +1627,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1895,8 +1949,8 @@
   <sheetPr/>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A53" sqref="$A53:$XFD64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -1907,11 +1961,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -3354,8 +3408,8 @@
   <sheetPr/>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -3623,7 +3677,7 @@
   <sheetPr/>
   <dimension ref="A1:XFD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -53117,4 +53171,151 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
+  <cols>
+    <col min="1" max="1" width="131.428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>